<commit_message>
Added Neural Network implementation
Has a bit issues with  neural network.
</commit_message>
<xml_diff>
--- a/Polynomial degree details.xlsx
+++ b/Polynomial degree details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ML\ML_PYTHON\projects\Music_Tagging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1188476-E690-4002-AC96-26A9DB3A7E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25D41E7-BCD2-4ECC-B634-2C9EBD73EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{52FA0481-E480-43D8-8624-E50D8675BBA8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>feature</t>
   </si>
@@ -39,88 +39,40 @@
     <t>alpha</t>
   </si>
   <si>
-    <t>final graph validity</t>
-  </si>
-  <si>
-    <t>Quality</t>
-  </si>
-  <si>
     <t>tempo</t>
   </si>
   <si>
     <t>Sr no</t>
   </si>
   <si>
-    <t>almost as expected</t>
-  </si>
-  <si>
-    <t>good, but not significant difference in J_error</t>
-  </si>
-  <si>
     <t>beats</t>
   </si>
   <si>
-    <t>optimal degree</t>
-  </si>
-  <si>
     <t>chroma_stft</t>
   </si>
   <si>
     <t>itr</t>
   </si>
   <si>
-    <t>,07</t>
-  </si>
-  <si>
-    <t>Not as expected</t>
-  </si>
-  <si>
-    <t>Not such a trust worthy feature</t>
-  </si>
-  <si>
     <t>rmse</t>
   </si>
   <si>
-    <t>Exactly as Expected</t>
-  </si>
-  <si>
-    <t>Might prove to be an extremely useful feature.</t>
-  </si>
-  <si>
     <t>spectral centroid</t>
   </si>
   <si>
-    <t xml:space="preserve">Might not provide any help and can create error </t>
-  </si>
-  <si>
     <t>spectral bandwidth</t>
   </si>
   <si>
-    <t>Not as Expected, as training error also increases</t>
-  </si>
-  <si>
-    <t>Mightnot prove to be very benefitial, but can be used</t>
-  </si>
-  <si>
     <t>rolloff</t>
   </si>
   <si>
-    <t>almost as expected, but training error is increasing</t>
-  </si>
-  <si>
-    <t>Might prove to be important,because val error is more than train err</t>
-  </si>
-  <si>
     <t>zero crossing rate</t>
   </si>
   <si>
-    <t xml:space="preserve">something nextto proper </t>
-  </si>
-  <si>
-    <t>Can prove to be a good feature</t>
-  </si>
-  <si>
-    <t>Exactly opposite of what expec+E6:E18ted</t>
+    <t>optimal deg</t>
+  </si>
+  <si>
+    <t>for 2 genre logistic</t>
   </si>
 </sst>
 </file>
@@ -168,13 +120,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B45441-ED2C-4306-9A80-B0010C2BAA32}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,285 +460,267 @@
     <col min="6" max="6" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="1">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>10000</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>10000</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="C10">
+        <v>10000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>1000</v>
-      </c>
-      <c r="D5">
-        <v>0.1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="D6" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8">
-        <v>1000</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4.9999999999999998E-7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>1000</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>26</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>